<commit_message>
move calendars to correct timezone
</commit_message>
<xml_diff>
--- a/app/static/example_data/embrace-plus_calendar_large.xlsx
+++ b/app/static/example_data/embrace-plus_calendar_large.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/veerlevanleemput/Documents/Hypebright BV/Fivoor/wearalyze/app/static/example_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2747CEAA-65AD-2945-9778-825B9BBD1DE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{938C04DD-E40B-5B42-A709-500EBC7BE388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3260" yWindow="1920" windowWidth="27640" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -460,7 +460,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -493,7 +493,7 @@
         <v>45118</v>
       </c>
       <c r="B2" s="2">
-        <v>0.32291666666666669</v>
+        <v>0.40972222222222227</v>
       </c>
       <c r="D2" t="s">
         <v>25</v>
@@ -507,7 +507,7 @@
         <v>45118</v>
       </c>
       <c r="B3" s="2">
-        <v>0.375</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="C3" s="2">
         <v>0.5</v>

</xml_diff>